<commit_message>
AutoCommit_22 сентября 2023 г. 12:59:55_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-222_Дискретная математика с элементами математической логики_I семестр.xlsx
+++ b/2ИСИП-222_Дискретная математика с элементами математической логики_I семестр.xlsx
@@ -19,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>2ИСИП-222: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
   <si>
-    <t>4сен</t>
-  </si>
-  <si>
-    <t>8сен</t>
-  </si>
-  <si>
     <t>11сен</t>
   </si>
   <si>
@@ -127,6 +121,12 @@
   </si>
   <si>
     <t>ОК</t>
+  </si>
+  <si>
+    <t>ДЗ2</t>
+  </si>
+  <si>
+    <t>ДЗ</t>
   </si>
 </sst>
 </file>
@@ -512,10 +512,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -552,16 +552,16 @@
     </row>
     <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="13" x14ac:dyDescent="0.25">
@@ -575,7 +575,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -587,12 +587,14 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
@@ -601,10 +603,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -615,10 +617,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -629,7 +631,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -641,7 +643,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -653,11 +655,11 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -667,7 +669,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -679,10 +681,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -693,11 +695,11 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -707,7 +709,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -719,10 +721,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -733,7 +735,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -745,7 +747,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -757,10 +759,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -771,9 +773,11 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -783,7 +787,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -797,7 +801,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -809,9 +813,11 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -821,7 +827,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -833,10 +839,10 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -847,7 +853,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -861,10 +867,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2">
@@ -877,7 +883,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -889,7 +895,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -901,7 +907,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -913,10 +919,10 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -927,7 +933,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -941,7 +947,7 @@
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>

</xml_diff>